<commit_message>
Documentación Fase 2 Completa
</commit_message>
<xml_diff>
--- a/FASE 1/DOCUMENTACIÓN PROYECTO/plantilla_product_backlog_puntos_historia.xlsx
+++ b/FASE 1/DOCUMENTACIÓN PROYECTO/plantilla_product_backlog_puntos_historia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victor\Desktop\manuela_info_pia_ISY\ISW\EXPERIENCIA_3\ACTIVIDAD_10\anexos\Product_backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jairo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91421A1-3B4B-4ACA-99DD-984EE293FD58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B45D3B0-E9D6-404E-A668-C7DFA9577CD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product_Backlog" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Product Backlog con estimación de historias</t>
   </si>
@@ -49,6 +52,33 @@
   </si>
   <si>
     <t>Total Puntos:</t>
+  </si>
+  <si>
+    <t>Autenticación</t>
+  </si>
+  <si>
+    <t>Registro de usuarios</t>
+  </si>
+  <si>
+    <t>Geolocalización</t>
+  </si>
+  <si>
+    <t>Agendar hora</t>
+  </si>
+  <si>
+    <t>Reporte de pagos</t>
+  </si>
+  <si>
+    <t>Registro de pago</t>
+  </si>
+  <si>
+    <t>Administrar talleres</t>
+  </si>
+  <si>
+    <t>Administrar vehículos</t>
+  </si>
+  <si>
+    <t>Cuenta de usuarios</t>
   </si>
 </sst>
 </file>
@@ -141,9 +171,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -153,13 +182,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,190 +475,244 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="54.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-    </row>
-    <row r="4" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <f>SUM(C7:C80)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="41.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" s="2"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>5</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>6</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>9</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>